<commit_message>
Update for repo-statistics spreadsheet
</commit_message>
<xml_diff>
--- a/data/repo-statistics.xlsx
+++ b/data/repo-statistics.xlsx
@@ -203,7 +203,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -252,8 +252,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -267,18 +275,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -611,7 +627,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection sqref="A1:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>